<commit_message>
Average Long.Strain variation per phase added, needs to be tested
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1051,16 +1051,16 @@
         <v>382</v>
       </c>
       <c r="U3" s="42" t="n">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="V3" s="42" t="n">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="W3" s="42" t="n">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="X3" s="43" t="n">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="Y3" s="43" t="n">
         <v>223</v>
@@ -1075,10 +1075,10 @@
         <v>652</v>
       </c>
       <c r="AC3" s="42" t="n">
-        <v>1016</v>
+        <v>1022</v>
       </c>
       <c r="AD3" s="42" t="n">
-        <v>1146</v>
+        <v>1149</v>
       </c>
       <c r="AE3" s="42" t="n">
         <v>1246</v>

</xml_diff>

<commit_message>
Improved the avgStrainVar function
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1051,16 +1051,16 @@
         <v>382</v>
       </c>
       <c r="U3" s="42" t="n">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="V3" s="42" t="n">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="W3" s="42" t="n">
-        <v>1149</v>
+        <v>1155</v>
       </c>
       <c r="X3" s="43" t="n">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="Y3" s="43" t="n">
         <v>223</v>
@@ -1075,10 +1075,10 @@
         <v>652</v>
       </c>
       <c r="AC3" s="42" t="n">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="AD3" s="42" t="n">
-        <v>1149</v>
+        <v>1155</v>
       </c>
       <c r="AE3" s="42" t="n">
         <v>1246</v>

</xml_diff>

<commit_message>
avgStrainVar plot is done
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1054,10 +1054,10 @@
         <v>107</v>
       </c>
       <c r="V3" s="42" t="n">
-        <v>1019</v>
+        <v>1004</v>
       </c>
       <c r="W3" s="42" t="n">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="X3" s="43" t="n">
         <v>107</v>
@@ -1075,10 +1075,10 @@
         <v>652</v>
       </c>
       <c r="AC3" s="42" t="n">
-        <v>1019</v>
+        <v>1004</v>
       </c>
       <c r="AD3" s="42" t="n">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="AE3" s="42" t="n">
         <v>1246</v>

</xml_diff>

<commit_message>
Added the SR from the strain in rawdatafiles.py
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1051,16 +1051,16 @@
         <v>382</v>
       </c>
       <c r="U3" s="42" t="n">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="V3" s="42" t="n">
-        <v>1004</v>
+        <v>1018</v>
       </c>
       <c r="W3" s="42" t="n">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="X3" s="43" t="n">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="Y3" s="43" t="n">
         <v>223</v>
@@ -1075,10 +1075,10 @@
         <v>652</v>
       </c>
       <c r="AC3" s="42" t="n">
-        <v>1004</v>
+        <v>1018</v>
       </c>
       <c r="AD3" s="42" t="n">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="AE3" s="42" t="n">
         <v>1246</v>

</xml_diff>

<commit_message>
verifies if there are ecg points selected - need to implement the plot
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1051,16 +1051,16 @@
         <v>382</v>
       </c>
       <c r="U3" s="42" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="V3" s="42" t="n">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="W3" s="42" t="n">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="X3" s="43" t="n">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Y3" s="43" t="n">
         <v>223</v>
@@ -1075,10 +1075,10 @@
         <v>652</v>
       </c>
       <c r="AC3" s="42" t="n">
-        <v>1018</v>
+        <v>1021</v>
       </c>
       <c r="AD3" s="42" t="n">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="AE3" s="42" t="n">
         <v>1246</v>

</xml_diff>

<commit_message>
added additional data from echopac to be shown
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -247,8 +247,8 @@
     <xf applyAlignment="1" borderId="0" fillId="10" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -320,8 +320,8 @@
     <xf applyAlignment="1" borderId="0" fillId="10" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -626,8 +626,8 @@
   </sheetPr>
   <dimension ref="A1:BI55"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
-      <selection activeCell="B47" activeCellId="0" pane="topLeft" sqref="B47"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="AJ1" view="normal" workbookViewId="0" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100">
+      <selection activeCell="AL2" activeCellId="0" pane="topLeft" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
@@ -720,12 +720,12 @@
       </c>
       <c r="AL1" s="35" t="inlineStr">
         <is>
-          <t>Parâmetros exportados do EchoPAC (4CH)</t>
+          <t>Exported from EchoPAC (4CH)</t>
         </is>
       </c>
       <c r="AX1" s="36" t="inlineStr">
         <is>
-          <t>Parâmetros exportados do EchoPAC (2CH)</t>
+          <t>Exported from EchoPAC (2CH)</t>
         </is>
       </c>
     </row>
@@ -1060,16 +1060,16 @@
         <v>382</v>
       </c>
       <c r="U3" s="44" t="n">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="V3" s="44" t="n">
-        <v>1021</v>
+        <v>1027</v>
       </c>
       <c r="W3" s="44" t="n">
-        <v>1146</v>
+        <v>1170</v>
       </c>
       <c r="X3" s="45" t="n">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="Y3" s="45" t="n">
         <v>223</v>
@@ -1084,10 +1084,10 @@
         <v>652</v>
       </c>
       <c r="AC3" s="44" t="n">
-        <v>1021</v>
+        <v>1027</v>
       </c>
       <c r="AD3" s="44" t="n">
-        <v>1146</v>
+        <v>1170</v>
       </c>
       <c r="AE3" s="44" t="n">
         <v>1246</v>
@@ -1102,13 +1102,13 @@
         <v>864</v>
       </c>
       <c r="AI3" s="46" t="n">
-        <v>0.4143518518518519</v>
+        <v>0.414351851851852</v>
       </c>
       <c r="AJ3" s="46" t="n">
         <v>-17.9</v>
       </c>
       <c r="AK3" s="46" t="n">
-        <v>36.6</v>
+        <v>38.4</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="4" s="29">
@@ -1177,7 +1177,7 @@
         <v>755</v>
       </c>
       <c r="AI4" s="46" t="n">
-        <v>0.5006622516556292</v>
+        <v>0.5006622516556291</v>
       </c>
       <c r="AJ4" s="46" t="n">
         <v>-7.4</v>
@@ -1321,10 +1321,10 @@
         <v>404</v>
       </c>
       <c r="AH5" s="45" t="n">
-        <v>807.9999999999999</v>
+        <v>808</v>
       </c>
       <c r="AI5" s="46" t="n">
-        <v>0.5000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="AJ5" s="46" t="n">
         <v>-11.6</v>
@@ -1394,13 +1394,13 @@
         <v>901</v>
       </c>
       <c r="AG6" s="45" t="n">
-        <v>-512.9999999999999</v>
+        <v>-513</v>
       </c>
       <c r="AH6" s="45" t="n">
         <v>1353</v>
       </c>
       <c r="AI6" s="46" t="n">
-        <v>-0.3791574279379157</v>
+        <v>-0.379157427937916</v>
       </c>
       <c r="AJ6" s="46" t="n">
         <v>-8.5</v>
@@ -1481,10 +1481,10 @@
         <v>0.604621309759064</v>
       </c>
       <c r="AJ7" s="50" t="n">
-        <v>-12.58</v>
+        <v>-12.6</v>
       </c>
       <c r="AK7" s="50" t="n">
-        <v>144.93</v>
+        <v>144.9</v>
       </c>
       <c r="AL7" s="44" t="n"/>
     </row>
@@ -1548,13 +1548,13 @@
         <v>1211</v>
       </c>
       <c r="AG8" s="45" t="n">
-        <v>-442.9999999999999</v>
+        <v>-443</v>
       </c>
       <c r="AH8" s="45" t="n">
         <v>1579</v>
       </c>
       <c r="AI8" s="46" t="n">
-        <v>-0.2805573147561748</v>
+        <v>-0.280557314756175</v>
       </c>
       <c r="AJ8" s="46" t="n">
         <v>-13.6</v>
@@ -1633,7 +1633,7 @@
         <v>1519</v>
       </c>
       <c r="AI9" s="46" t="n">
-        <v>-0.3238973008558262</v>
+        <v>-0.323897300855826</v>
       </c>
       <c r="AJ9" s="46" t="n">
         <v>-18.3</v>
@@ -1703,13 +1703,13 @@
         <v>908</v>
       </c>
       <c r="AG10" s="45" t="n">
-        <v>-388.0000000000001</v>
+        <v>-388</v>
       </c>
       <c r="AH10" s="45" t="n">
         <v>1205</v>
       </c>
       <c r="AI10" s="46" t="n">
-        <v>-0.3219917012448133</v>
+        <v>-0.321991701244813</v>
       </c>
       <c r="AJ10" s="46" t="n">
         <v>-4.6</v>
@@ -1779,7 +1779,7 @@
         <v>849</v>
       </c>
       <c r="AG11" s="45" t="n">
-        <v>-362.0000000000001</v>
+        <v>-362</v>
       </c>
       <c r="AH11" s="45" t="n">
         <v>1173</v>
@@ -1861,7 +1861,7 @@
         <v>774</v>
       </c>
       <c r="AI12" s="46" t="n">
-        <v>0.4483204134366925</v>
+        <v>0.448320413436692</v>
       </c>
       <c r="AJ12" s="46" t="n">
         <v>-16.3</v>
@@ -1937,7 +1937,7 @@
         <v>1366</v>
       </c>
       <c r="AI13" s="46" t="n">
-        <v>-0.3433382137628111</v>
+        <v>-0.343338213762811</v>
       </c>
       <c r="AJ13" s="46" t="n">
         <v>-11.6</v>
@@ -2089,7 +2089,7 @@
         <v>891</v>
       </c>
       <c r="AI15" s="46" t="n">
-        <v>0.4365881032547699</v>
+        <v>0.43658810325477</v>
       </c>
       <c r="AJ15" s="46" t="n">
         <v>-7.3</v>
@@ -2165,7 +2165,7 @@
         <v>591</v>
       </c>
       <c r="AI16" s="46" t="n">
-        <v>0.6192893401015228</v>
+        <v>0.619289340101523</v>
       </c>
       <c r="AJ16" s="46" t="n">
         <v>-17.4</v>
@@ -2241,7 +2241,7 @@
         <v>1574</v>
       </c>
       <c r="AI17" s="46" t="n">
-        <v>-0.3310038119440915</v>
+        <v>-0.331003811944091</v>
       </c>
       <c r="AJ17" s="46" t="n">
         <v>-20.2</v>
@@ -2317,7 +2317,7 @@
         <v>1575</v>
       </c>
       <c r="AI18" s="46" t="n">
-        <v>-0.3498412698412698</v>
+        <v>-0.34984126984127</v>
       </c>
       <c r="AJ18" s="46" t="n">
         <v>-19.6</v>
@@ -2390,10 +2390,10 @@
         <v>372</v>
       </c>
       <c r="AH19" s="45" t="n">
-        <v>948.0000000000001</v>
+        <v>948</v>
       </c>
       <c r="AI19" s="46" t="n">
-        <v>0.3924050632911392</v>
+        <v>0.392405063291139</v>
       </c>
       <c r="AJ19" s="46" t="n">
         <v>-15.1</v>
@@ -2463,13 +2463,13 @@
         <v>1048</v>
       </c>
       <c r="AG20" s="45" t="n">
-        <v>-674.9999999999999</v>
+        <v>-675</v>
       </c>
       <c r="AH20" s="45" t="n">
         <v>1645</v>
       </c>
       <c r="AI20" s="46" t="n">
-        <v>-0.4103343465045592</v>
+        <v>-0.410334346504559</v>
       </c>
       <c r="AJ20" s="46" t="n">
         <v>-19.3</v>
@@ -2545,7 +2545,7 @@
         <v>966</v>
       </c>
       <c r="AI21" s="46" t="n">
-        <v>0.3799171842650104</v>
+        <v>0.37991718426501</v>
       </c>
       <c r="AJ21" s="46" t="n">
         <v>-19.1</v>
@@ -2655,16 +2655,16 @@
         <v>354</v>
       </c>
       <c r="U23" s="46" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="V23" s="46" t="n">
-        <v>1170</v>
+        <v>1034</v>
       </c>
       <c r="W23" s="46" t="n">
-        <v>1039</v>
+        <v>1167</v>
       </c>
       <c r="X23" s="45" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="Y23" s="45" t="n">
         <v>996</v>
@@ -2679,10 +2679,10 @@
         <v>599</v>
       </c>
       <c r="AC23" s="46" t="n">
-        <v>1170</v>
+        <v>1034</v>
       </c>
       <c r="AD23" s="46" t="n">
-        <v>1039</v>
+        <v>1167</v>
       </c>
       <c r="AE23" s="46" t="n">
         <v>2037</v>
@@ -2703,7 +2703,7 @@
         <v>-16.7</v>
       </c>
       <c r="AK23" s="46" t="n">
-        <v>57.7</v>
+        <v>99.59999999999999</v>
       </c>
       <c r="AL23" s="46" t="n"/>
     </row>
@@ -2773,7 +2773,7 @@
         <v>1001</v>
       </c>
       <c r="AI24" s="46" t="n">
-        <v>0.3536463536463537</v>
+        <v>0.353646353646354</v>
       </c>
       <c r="AJ24" s="46" t="n">
         <v>-19.8</v>
@@ -2843,13 +2843,13 @@
         <v>2290</v>
       </c>
       <c r="AG25" s="45" t="n">
-        <v>322.0000000000001</v>
+        <v>322</v>
       </c>
       <c r="AH25" s="45" t="n">
         <v>883</v>
       </c>
       <c r="AI25" s="46" t="n">
-        <v>0.3646659116647792</v>
+        <v>0.364665911664779</v>
       </c>
       <c r="AJ25" s="46" t="n">
         <v>-16</v>
@@ -2919,13 +2919,13 @@
         <v>1130</v>
       </c>
       <c r="AG26" s="45" t="n">
-        <v>420.9999999999999</v>
+        <v>421</v>
       </c>
       <c r="AH26" s="45" t="n">
         <v>646</v>
       </c>
       <c r="AI26" s="46" t="n">
-        <v>0.6517027863777088</v>
+        <v>0.651702786377709</v>
       </c>
       <c r="AJ26" s="46" t="n">
         <v>-20.8</v>
@@ -2995,13 +2995,13 @@
         <v>1091</v>
       </c>
       <c r="AG27" s="45" t="n">
-        <v>-508.9999999999999</v>
+        <v>-509</v>
       </c>
       <c r="AH27" s="45" t="n">
         <v>1562</v>
       </c>
       <c r="AI27" s="46" t="n">
-        <v>-0.3258642765685019</v>
+        <v>-0.325864276568502</v>
       </c>
       <c r="AJ27" s="46" t="n">
         <v>-14.7</v>
@@ -3077,7 +3077,7 @@
         <v>1695</v>
       </c>
       <c r="AI28" s="46" t="n">
-        <v>-0.3746312684365782</v>
+        <v>-0.374631268436578</v>
       </c>
       <c r="AJ28" s="46" t="n">
         <v>-19.9</v>
@@ -3147,13 +3147,13 @@
         <v>1136</v>
       </c>
       <c r="AG29" s="45" t="n">
-        <v>358.0000000000001</v>
+        <v>358</v>
       </c>
       <c r="AH29" s="45" t="n">
         <v>704</v>
       </c>
       <c r="AI29" s="46" t="n">
-        <v>0.5085227272727274</v>
+        <v>0.508522727272727</v>
       </c>
       <c r="AJ29" s="46" t="n">
         <v>-18.1</v>
@@ -3223,13 +3223,13 @@
         <v>1004</v>
       </c>
       <c r="AG30" s="45" t="n">
-        <v>-417.9999999999999</v>
+        <v>-418</v>
       </c>
       <c r="AH30" s="45" t="n">
         <v>1362</v>
       </c>
       <c r="AI30" s="46" t="n">
-        <v>-0.3069016152716593</v>
+        <v>-0.306901615271659</v>
       </c>
       <c r="AJ30" s="46" t="n">
         <v>-20.4</v>
@@ -3299,13 +3299,13 @@
         <v>874</v>
       </c>
       <c r="AG31" s="45" t="n">
-        <v>-424.0000000000001</v>
+        <v>-424</v>
       </c>
       <c r="AH31" s="45" t="n">
         <v>1237</v>
       </c>
       <c r="AI31" s="46" t="n">
-        <v>-0.3427647534357316</v>
+        <v>-0.342764753435732</v>
       </c>
       <c r="AJ31" s="46" t="n">
         <v>-17.5</v>
@@ -3378,10 +3378,10 @@
         <v>377</v>
       </c>
       <c r="AH32" s="46" t="n">
-        <v>951.0000000000001</v>
+        <v>951</v>
       </c>
       <c r="AI32" s="46" t="n">
-        <v>0.3964248159831756</v>
+        <v>0.396424815983176</v>
       </c>
       <c r="AJ32" s="46" t="n">
         <v>-17</v>
@@ -3474,7 +3474,7 @@
         <v>971</v>
       </c>
       <c r="AI33" s="51" t="n">
-        <v>0.3542739443872296</v>
+        <v>0.35427394438723</v>
       </c>
       <c r="AJ33" s="46" t="n">
         <v>-21.2</v>
@@ -3550,7 +3550,7 @@
         <v>1182</v>
       </c>
       <c r="AI34" s="51" t="n">
-        <v>0.3147208121827411</v>
+        <v>0.314720812182741</v>
       </c>
       <c r="AJ34" s="46" t="n">
         <v>-23.1</v>
@@ -3620,13 +3620,13 @@
         <v>1293</v>
       </c>
       <c r="AG35" s="51" t="n">
-        <v>340.9999999999999</v>
+        <v>341</v>
       </c>
       <c r="AH35" s="51" t="n">
-        <v>868.0000000000001</v>
+        <v>868</v>
       </c>
       <c r="AI35" s="51" t="n">
-        <v>0.3928571428571427</v>
+        <v>0.392857142857143</v>
       </c>
       <c r="AJ35" s="46" t="n">
         <v>-19.9</v>
@@ -3696,13 +3696,13 @@
         <v>1310</v>
       </c>
       <c r="AG36" s="51" t="n">
-        <v>386.0000000000001</v>
+        <v>386</v>
       </c>
       <c r="AH36" s="51" t="n">
         <v>843</v>
       </c>
       <c r="AI36" s="51" t="n">
-        <v>0.4578884934756822</v>
+        <v>0.457888493475682</v>
       </c>
       <c r="AJ36" s="46" t="n">
         <v>-21.2</v>
@@ -3772,13 +3772,13 @@
         <v>1197</v>
       </c>
       <c r="AG37" s="51" t="n">
-        <v>358.0000000000001</v>
+        <v>358</v>
       </c>
       <c r="AH37" s="51" t="n">
         <v>758</v>
       </c>
       <c r="AI37" s="51" t="n">
-        <v>0.4722955145118735</v>
+        <v>0.472295514511873</v>
       </c>
       <c r="AJ37" s="46" t="n">
         <v>-24.6</v>
@@ -3854,7 +3854,7 @@
         <v>810</v>
       </c>
       <c r="AI38" s="51" t="n">
-        <v>0.4432098765432098</v>
+        <v>0.44320987654321</v>
       </c>
       <c r="AJ38" s="46" t="n">
         <v>-19.6</v>
@@ -3930,7 +3930,7 @@
         <v>1021</v>
       </c>
       <c r="AI39" s="51" t="n">
-        <v>0.3917727717923605</v>
+        <v>0.39177277179236</v>
       </c>
       <c r="AJ39" s="46" t="n">
         <v>-7.1</v>
@@ -4003,10 +4003,10 @@
         <v>177</v>
       </c>
       <c r="AH40" s="51" t="n">
-        <v>552.9999999999999</v>
+        <v>553</v>
       </c>
       <c r="AI40" s="51" t="n">
-        <v>0.3200723327305606</v>
+        <v>0.320072332730561</v>
       </c>
       <c r="AJ40" s="46" t="n">
         <v>-4.2</v>
@@ -4079,10 +4079,10 @@
         <v>266</v>
       </c>
       <c r="AH41" s="51" t="n">
-        <v>437.9999999999999</v>
+        <v>438</v>
       </c>
       <c r="AI41" s="51" t="n">
-        <v>0.6073059360730595</v>
+        <v>0.607305936073059</v>
       </c>
       <c r="AJ41" s="46" t="n">
         <v>-5.3</v>
@@ -4158,7 +4158,7 @@
         <v>1074</v>
       </c>
       <c r="AI42" s="51" t="n">
-        <v>0.3398510242085661</v>
+        <v>0.339851024208566</v>
       </c>
       <c r="AJ42" s="46" t="n">
         <v>-4.4</v>
@@ -4227,13 +4227,13 @@
         <v>1127</v>
       </c>
       <c r="AG43" s="51" t="n">
-        <v>359.0000000000001</v>
+        <v>359</v>
       </c>
       <c r="AH43" s="51" t="n">
-        <v>595.9999999999999</v>
+        <v>596</v>
       </c>
       <c r="AI43" s="51" t="n">
-        <v>0.6023489932885908</v>
+        <v>0.602348993288591</v>
       </c>
       <c r="AJ43" s="46" t="n">
         <v>-10.6</v>
@@ -4303,13 +4303,13 @@
         <v>1390</v>
       </c>
       <c r="AG44" s="51" t="n">
-        <v>408.0000000000001</v>
+        <v>408</v>
       </c>
       <c r="AH44" s="51" t="n">
-        <v>795.9999999999999</v>
+        <v>796</v>
       </c>
       <c r="AI44" s="51" t="n">
-        <v>0.5125628140703519</v>
+        <v>0.512562814070352</v>
       </c>
       <c r="AJ44" s="46" t="n">
         <v>-11.6</v>
@@ -4446,13 +4446,13 @@
         <v>801</v>
       </c>
       <c r="AG46" s="51" t="n">
-        <v>317.0000000000001</v>
+        <v>317</v>
       </c>
       <c r="AH46" s="51" t="n">
-        <v>426.9999999999999</v>
+        <v>427</v>
       </c>
       <c r="AI46" s="51" t="n">
-        <v>0.7423887587822017</v>
+        <v>0.742388758782202</v>
       </c>
       <c r="AJ46" s="46" t="n">
         <v>-11.1</v>
@@ -4528,7 +4528,7 @@
         <v>745</v>
       </c>
       <c r="AI47" s="51" t="n">
-        <v>0.3718120805369128</v>
+        <v>0.371812080536913</v>
       </c>
       <c r="AJ47" s="46" t="n">
         <v>-3.8</v>
@@ -4604,7 +4604,7 @@
         <v>898</v>
       </c>
       <c r="AI48" s="51" t="n">
-        <v>0.3853006681514476</v>
+        <v>0.385300668151448</v>
       </c>
       <c r="AJ48" s="46" t="n">
         <v>-8.699999999999999</v>
@@ -4769,10 +4769,10 @@
         <v>312</v>
       </c>
       <c r="AH50" s="46" t="n">
-        <v>829.9999999999999</v>
+        <v>830</v>
       </c>
       <c r="AI50" s="46" t="n">
-        <v>0.3759036144578314</v>
+        <v>0.375903614457831</v>
       </c>
       <c r="AJ50" s="46" t="n">
         <v>-6.6</v>
@@ -4848,7 +4848,7 @@
         <v>504</v>
       </c>
       <c r="AI51" s="46" t="n">
-        <v>0.7440476190476191</v>
+        <v>0.744047619047619</v>
       </c>
       <c r="AJ51" s="46" t="n">
         <v>-10.8</v>
@@ -4921,10 +4921,10 @@
         <v>390</v>
       </c>
       <c r="AH52" s="46" t="n">
-        <v>460.9999999999999</v>
+        <v>461</v>
       </c>
       <c r="AI52" s="46" t="n">
-        <v>0.8459869848156183</v>
+        <v>0.845986984815618</v>
       </c>
       <c r="AJ52" s="46" t="n">
         <v>-9.6</v>

</xml_diff>

<commit_message>
Peak systolic strain detection added
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1102,7 +1102,7 @@
         <v>864</v>
       </c>
       <c r="AI3" s="46" t="n">
-        <v>0.414351851851852</v>
+        <v>0.4143518518518519</v>
       </c>
       <c r="AJ3" s="46" t="n">
         <v>-17.9</v>
@@ -1177,13 +1177,13 @@
         <v>755</v>
       </c>
       <c r="AI4" s="46" t="n">
-        <v>0.5006622516556291</v>
+        <v>0.5006622516556292</v>
       </c>
       <c r="AJ4" s="46" t="n">
-        <v>-7.4</v>
+        <v>-6.7</v>
       </c>
       <c r="AK4" s="46" t="n">
-        <v>87.5</v>
+        <v>118.7</v>
       </c>
       <c r="AL4" s="28" t="n">
         <v>1</v>
@@ -1282,16 +1282,16 @@
         <v>441</v>
       </c>
       <c r="U5" s="44" t="n">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="V5" s="44" t="n">
-        <v>1105</v>
+        <v>964</v>
       </c>
       <c r="W5" s="44" t="n">
-        <v>949</v>
+        <v>1176</v>
       </c>
       <c r="X5" s="45" t="n">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="Y5" s="45" t="n">
         <v>230</v>
@@ -1306,10 +1306,10 @@
         <v>718</v>
       </c>
       <c r="AC5" s="46" t="n">
-        <v>1105</v>
+        <v>964</v>
       </c>
       <c r="AD5" s="46" t="n">
-        <v>949</v>
+        <v>1176</v>
       </c>
       <c r="AE5" s="46" t="n">
         <v>1249</v>
@@ -1321,16 +1321,16 @@
         <v>404</v>
       </c>
       <c r="AH5" s="45" t="n">
-        <v>808</v>
+        <v>807.9999999999999</v>
       </c>
       <c r="AI5" s="46" t="n">
-        <v>0.5</v>
+        <v>0.5000000000000001</v>
       </c>
       <c r="AJ5" s="46" t="n">
-        <v>-11.6</v>
+        <v>-10.6</v>
       </c>
       <c r="AK5" s="46" t="n">
-        <v>81.40000000000001</v>
+        <v>108</v>
       </c>
       <c r="AL5" s="44" t="n"/>
     </row>
@@ -1394,19 +1394,19 @@
         <v>901</v>
       </c>
       <c r="AG6" s="45" t="n">
-        <v>-513</v>
+        <v>-512.9999999999999</v>
       </c>
       <c r="AH6" s="45" t="n">
         <v>1353</v>
       </c>
       <c r="AI6" s="46" t="n">
-        <v>-0.379157427937916</v>
+        <v>-0.3791574279379157</v>
       </c>
       <c r="AJ6" s="46" t="n">
-        <v>-8.5</v>
+        <v>-8.4</v>
       </c>
       <c r="AK6" s="46" t="n">
-        <v>83.2</v>
+        <v>89.8</v>
       </c>
       <c r="AL6" s="44" t="n"/>
     </row>
@@ -1548,19 +1548,19 @@
         <v>1211</v>
       </c>
       <c r="AG8" s="45" t="n">
-        <v>-443</v>
+        <v>-442.9999999999999</v>
       </c>
       <c r="AH8" s="45" t="n">
         <v>1579</v>
       </c>
       <c r="AI8" s="46" t="n">
-        <v>-0.280557314756175</v>
+        <v>-0.2805573147561748</v>
       </c>
       <c r="AJ8" s="46" t="n">
         <v>-13.6</v>
       </c>
       <c r="AK8" s="46" t="n">
-        <v>75.7</v>
+        <v>80.7</v>
       </c>
       <c r="AL8" s="44" t="n"/>
       <c r="BD8" s="27" t="n"/>
@@ -1633,7 +1633,7 @@
         <v>1519</v>
       </c>
       <c r="AI9" s="46" t="n">
-        <v>-0.323897300855826</v>
+        <v>-0.3238973008558262</v>
       </c>
       <c r="AJ9" s="46" t="n">
         <v>-18.3</v>
@@ -1703,19 +1703,19 @@
         <v>908</v>
       </c>
       <c r="AG10" s="45" t="n">
-        <v>-388</v>
+        <v>-388.0000000000001</v>
       </c>
       <c r="AH10" s="45" t="n">
         <v>1205</v>
       </c>
       <c r="AI10" s="46" t="n">
-        <v>-0.321991701244813</v>
+        <v>-0.3219917012448133</v>
       </c>
       <c r="AJ10" s="46" t="n">
-        <v>-4.6</v>
+        <v>-2.5</v>
       </c>
       <c r="AK10" s="46" t="n">
-        <v>91.3</v>
+        <v>123.7</v>
       </c>
       <c r="AL10" s="44" t="n"/>
     </row>
@@ -1779,7 +1779,7 @@
         <v>849</v>
       </c>
       <c r="AG11" s="45" t="n">
-        <v>-362</v>
+        <v>-362.0000000000001</v>
       </c>
       <c r="AH11" s="45" t="n">
         <v>1173</v>
@@ -1861,7 +1861,7 @@
         <v>774</v>
       </c>
       <c r="AI12" s="46" t="n">
-        <v>0.448320413436692</v>
+        <v>0.4483204134366925</v>
       </c>
       <c r="AJ12" s="46" t="n">
         <v>-16.3</v>
@@ -1937,13 +1937,13 @@
         <v>1366</v>
       </c>
       <c r="AI13" s="46" t="n">
-        <v>-0.343338213762811</v>
+        <v>-0.3433382137628111</v>
       </c>
       <c r="AJ13" s="46" t="n">
-        <v>-11.6</v>
+        <v>-11.2</v>
       </c>
       <c r="AK13" s="46" t="n">
-        <v>51.2</v>
+        <v>59.6</v>
       </c>
       <c r="AL13" s="44" t="n"/>
     </row>
@@ -2047,16 +2047,16 @@
         <v>399</v>
       </c>
       <c r="U15" s="44" t="n">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="V15" s="44" t="n">
-        <v>1179</v>
+        <v>1088</v>
       </c>
       <c r="W15" s="44" t="n">
-        <v>1063</v>
+        <v>1254</v>
       </c>
       <c r="X15" s="45" t="n">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="Y15" s="45" t="n">
         <v>223</v>
@@ -2071,10 +2071,10 @@
         <v>696</v>
       </c>
       <c r="AC15" s="46" t="n">
-        <v>1179</v>
+        <v>1088</v>
       </c>
       <c r="AD15" s="46" t="n">
-        <v>1063</v>
+        <v>1254</v>
       </c>
       <c r="AE15" s="46" t="n">
         <v>1290</v>
@@ -2089,13 +2089,13 @@
         <v>891</v>
       </c>
       <c r="AI15" s="46" t="n">
-        <v>0.43658810325477</v>
+        <v>0.4365881032547699</v>
       </c>
       <c r="AJ15" s="46" t="n">
         <v>-7.3</v>
       </c>
       <c r="AK15" s="46" t="n">
-        <v>39.7</v>
+        <v>103.2</v>
       </c>
       <c r="AL15" s="44" t="n"/>
     </row>
@@ -2165,13 +2165,13 @@
         <v>591</v>
       </c>
       <c r="AI16" s="46" t="n">
-        <v>0.619289340101523</v>
+        <v>0.6192893401015228</v>
       </c>
       <c r="AJ16" s="46" t="n">
         <v>-17.4</v>
       </c>
       <c r="AK16" s="46" t="n">
-        <v>34.2</v>
+        <v>38.4</v>
       </c>
       <c r="AL16" s="46" t="n"/>
     </row>
@@ -2241,13 +2241,13 @@
         <v>1574</v>
       </c>
       <c r="AI17" s="46" t="n">
-        <v>-0.331003811944091</v>
+        <v>-0.3310038119440915</v>
       </c>
       <c r="AJ17" s="46" t="n">
         <v>-20.2</v>
       </c>
       <c r="AK17" s="46" t="n">
-        <v>43.4</v>
+        <v>42.7</v>
       </c>
       <c r="AL17" s="46" t="n"/>
     </row>
@@ -2317,13 +2317,13 @@
         <v>1575</v>
       </c>
       <c r="AI18" s="46" t="n">
-        <v>-0.34984126984127</v>
+        <v>-0.3498412698412698</v>
       </c>
       <c r="AJ18" s="46" t="n">
         <v>-19.6</v>
       </c>
       <c r="AK18" s="46" t="n">
-        <v>35.7</v>
+        <v>39.1</v>
       </c>
       <c r="AL18" s="46" t="n"/>
     </row>
@@ -2390,10 +2390,10 @@
         <v>372</v>
       </c>
       <c r="AH19" s="45" t="n">
-        <v>948</v>
+        <v>948.0000000000001</v>
       </c>
       <c r="AI19" s="46" t="n">
-        <v>0.392405063291139</v>
+        <v>0.3924050632911392</v>
       </c>
       <c r="AJ19" s="46" t="n">
         <v>-15.1</v>
@@ -2463,19 +2463,19 @@
         <v>1048</v>
       </c>
       <c r="AG20" s="45" t="n">
-        <v>-675</v>
+        <v>-674.9999999999999</v>
       </c>
       <c r="AH20" s="45" t="n">
         <v>1645</v>
       </c>
       <c r="AI20" s="46" t="n">
-        <v>-0.410334346504559</v>
+        <v>-0.4103343465045592</v>
       </c>
       <c r="AJ20" s="46" t="n">
         <v>-19.3</v>
       </c>
       <c r="AK20" s="46" t="n">
-        <v>23.9</v>
+        <v>91.90000000000001</v>
       </c>
       <c r="AL20" s="46" t="n"/>
     </row>
@@ -2545,13 +2545,13 @@
         <v>966</v>
       </c>
       <c r="AI21" s="46" t="n">
-        <v>0.37991718426501</v>
+        <v>0.3799171842650104</v>
       </c>
       <c r="AJ21" s="46" t="n">
         <v>-19.1</v>
       </c>
       <c r="AK21" s="46" t="n">
-        <v>52.2</v>
+        <v>51.4</v>
       </c>
       <c r="AL21" s="46" t="n"/>
     </row>
@@ -2627,7 +2627,7 @@
         <v>-16.9</v>
       </c>
       <c r="AK22" s="46" t="n">
-        <v>53.7</v>
+        <v>53</v>
       </c>
       <c r="AL22" s="46" t="n"/>
     </row>
@@ -2773,13 +2773,13 @@
         <v>1001</v>
       </c>
       <c r="AI24" s="46" t="n">
-        <v>0.353646353646354</v>
+        <v>0.3536463536463537</v>
       </c>
       <c r="AJ24" s="46" t="n">
         <v>-19.8</v>
       </c>
       <c r="AK24" s="46" t="n">
-        <v>30.3</v>
+        <v>37.9</v>
       </c>
       <c r="AL24" s="46" t="n"/>
     </row>
@@ -2843,19 +2843,19 @@
         <v>2290</v>
       </c>
       <c r="AG25" s="45" t="n">
-        <v>322</v>
+        <v>322.0000000000001</v>
       </c>
       <c r="AH25" s="45" t="n">
         <v>883</v>
       </c>
       <c r="AI25" s="46" t="n">
-        <v>0.364665911664779</v>
+        <v>0.3646659116647792</v>
       </c>
       <c r="AJ25" s="46" t="n">
         <v>-16</v>
       </c>
       <c r="AK25" s="46" t="n">
-        <v>51.7</v>
+        <v>70.40000000000001</v>
       </c>
       <c r="AL25" s="46" t="n"/>
     </row>
@@ -2919,19 +2919,19 @@
         <v>1130</v>
       </c>
       <c r="AG26" s="45" t="n">
-        <v>421</v>
+        <v>420.9999999999999</v>
       </c>
       <c r="AH26" s="45" t="n">
         <v>646</v>
       </c>
       <c r="AI26" s="46" t="n">
-        <v>0.651702786377709</v>
+        <v>0.6517027863777088</v>
       </c>
       <c r="AJ26" s="46" t="n">
         <v>-20.8</v>
       </c>
       <c r="AK26" s="46" t="n">
-        <v>39.9</v>
+        <v>42.7</v>
       </c>
       <c r="AL26" s="46" t="n"/>
     </row>
@@ -2995,19 +2995,19 @@
         <v>1091</v>
       </c>
       <c r="AG27" s="45" t="n">
-        <v>-509</v>
+        <v>-508.9999999999999</v>
       </c>
       <c r="AH27" s="45" t="n">
         <v>1562</v>
       </c>
       <c r="AI27" s="46" t="n">
-        <v>-0.325864276568502</v>
+        <v>-0.3258642765685019</v>
       </c>
       <c r="AJ27" s="46" t="n">
         <v>-14.7</v>
       </c>
       <c r="AK27" s="46" t="n">
-        <v>55.1</v>
+        <v>85</v>
       </c>
       <c r="AL27" s="46" t="n"/>
     </row>
@@ -3077,13 +3077,13 @@
         <v>1695</v>
       </c>
       <c r="AI28" s="46" t="n">
-        <v>-0.374631268436578</v>
+        <v>-0.3746312684365782</v>
       </c>
       <c r="AJ28" s="46" t="n">
         <v>-19.9</v>
       </c>
       <c r="AK28" s="46" t="n">
-        <v>36.3</v>
+        <v>104.5</v>
       </c>
       <c r="AL28" s="46" t="n"/>
     </row>
@@ -3147,19 +3147,19 @@
         <v>1136</v>
       </c>
       <c r="AG29" s="45" t="n">
-        <v>358</v>
+        <v>358.0000000000001</v>
       </c>
       <c r="AH29" s="45" t="n">
         <v>704</v>
       </c>
       <c r="AI29" s="46" t="n">
-        <v>0.508522727272727</v>
+        <v>0.5085227272727274</v>
       </c>
       <c r="AJ29" s="46" t="n">
         <v>-18.1</v>
       </c>
       <c r="AK29" s="46" t="n">
-        <v>29.9</v>
+        <v>81.2</v>
       </c>
       <c r="AL29" s="46" t="n"/>
     </row>
@@ -3223,19 +3223,19 @@
         <v>1004</v>
       </c>
       <c r="AG30" s="45" t="n">
-        <v>-418</v>
+        <v>-417.9999999999999</v>
       </c>
       <c r="AH30" s="45" t="n">
         <v>1362</v>
       </c>
       <c r="AI30" s="46" t="n">
-        <v>-0.306901615271659</v>
+        <v>-0.3069016152716593</v>
       </c>
       <c r="AJ30" s="46" t="n">
         <v>-20.4</v>
       </c>
       <c r="AK30" s="46" t="n">
-        <v>52.4</v>
+        <v>54.5</v>
       </c>
       <c r="AL30" s="46" t="n"/>
     </row>
@@ -3299,13 +3299,13 @@
         <v>874</v>
       </c>
       <c r="AG31" s="45" t="n">
-        <v>-424</v>
+        <v>-424.0000000000001</v>
       </c>
       <c r="AH31" s="45" t="n">
         <v>1237</v>
       </c>
       <c r="AI31" s="46" t="n">
-        <v>-0.342764753435732</v>
+        <v>-0.3427647534357316</v>
       </c>
       <c r="AJ31" s="46" t="n">
         <v>-17.5</v>
@@ -3378,16 +3378,16 @@
         <v>377</v>
       </c>
       <c r="AH32" s="46" t="n">
-        <v>951</v>
+        <v>951.0000000000001</v>
       </c>
       <c r="AI32" s="46" t="n">
-        <v>0.396424815983176</v>
+        <v>0.3964248159831756</v>
       </c>
       <c r="AJ32" s="46" t="n">
         <v>-17</v>
       </c>
       <c r="AK32" s="46" t="n">
-        <v>28.1</v>
+        <v>30.6</v>
       </c>
       <c r="AL32" s="45" t="n"/>
       <c r="AM32" s="46" t="n"/>
@@ -3474,7 +3474,7 @@
         <v>971</v>
       </c>
       <c r="AI33" s="51" t="n">
-        <v>0.35427394438723</v>
+        <v>0.3542739443872296</v>
       </c>
       <c r="AJ33" s="46" t="n">
         <v>-21.2</v>
@@ -3550,13 +3550,13 @@
         <v>1182</v>
       </c>
       <c r="AI34" s="51" t="n">
-        <v>0.314720812182741</v>
+        <v>0.3147208121827411</v>
       </c>
       <c r="AJ34" s="46" t="n">
         <v>-23.1</v>
       </c>
       <c r="AK34" s="46" t="n">
-        <v>39.6</v>
+        <v>38.7</v>
       </c>
       <c r="AL34" s="45" t="n"/>
     </row>
@@ -3620,19 +3620,19 @@
         <v>1293</v>
       </c>
       <c r="AG35" s="51" t="n">
-        <v>341</v>
+        <v>340.9999999999999</v>
       </c>
       <c r="AH35" s="51" t="n">
-        <v>868</v>
+        <v>868.0000000000001</v>
       </c>
       <c r="AI35" s="51" t="n">
-        <v>0.392857142857143</v>
+        <v>0.3928571428571427</v>
       </c>
       <c r="AJ35" s="46" t="n">
         <v>-19.9</v>
       </c>
       <c r="AK35" s="46" t="n">
-        <v>27.3</v>
+        <v>25.6</v>
       </c>
       <c r="AL35" s="45" t="n"/>
     </row>
@@ -3696,19 +3696,19 @@
         <v>1310</v>
       </c>
       <c r="AG36" s="51" t="n">
-        <v>386</v>
+        <v>386.0000000000001</v>
       </c>
       <c r="AH36" s="51" t="n">
         <v>843</v>
       </c>
       <c r="AI36" s="51" t="n">
-        <v>0.457888493475682</v>
+        <v>0.4578884934756822</v>
       </c>
       <c r="AJ36" s="46" t="n">
         <v>-21.2</v>
       </c>
       <c r="AK36" s="46" t="n">
-        <v>34.7</v>
+        <v>41.3</v>
       </c>
       <c r="AL36" s="45" t="n"/>
     </row>
@@ -3772,13 +3772,13 @@
         <v>1197</v>
       </c>
       <c r="AG37" s="51" t="n">
-        <v>358</v>
+        <v>358.0000000000001</v>
       </c>
       <c r="AH37" s="51" t="n">
         <v>758</v>
       </c>
       <c r="AI37" s="51" t="n">
-        <v>0.472295514511873</v>
+        <v>0.4722955145118735</v>
       </c>
       <c r="AJ37" s="46" t="n">
         <v>-24.6</v>
@@ -3854,13 +3854,13 @@
         <v>810</v>
       </c>
       <c r="AI38" s="51" t="n">
-        <v>0.44320987654321</v>
+        <v>0.4432098765432098</v>
       </c>
       <c r="AJ38" s="46" t="n">
         <v>-19.6</v>
       </c>
       <c r="AK38" s="46" t="n">
-        <v>35.4</v>
+        <v>37.1</v>
       </c>
       <c r="AL38" s="45" t="n"/>
     </row>
@@ -3930,13 +3930,13 @@
         <v>1021</v>
       </c>
       <c r="AI39" s="51" t="n">
-        <v>0.39177277179236</v>
+        <v>0.3917727717923605</v>
       </c>
       <c r="AJ39" s="46" t="n">
-        <v>-7.1</v>
+        <v>-6.4</v>
       </c>
       <c r="AK39" s="46" t="n">
-        <v>73.40000000000001</v>
+        <v>62.2</v>
       </c>
       <c r="AL39" s="45" t="n"/>
     </row>
@@ -4003,16 +4003,16 @@
         <v>177</v>
       </c>
       <c r="AH40" s="51" t="n">
-        <v>553</v>
+        <v>552.9999999999999</v>
       </c>
       <c r="AI40" s="51" t="n">
-        <v>0.320072332730561</v>
+        <v>0.3200723327305606</v>
       </c>
       <c r="AJ40" s="46" t="n">
-        <v>-4.2</v>
+        <v>-3.8</v>
       </c>
       <c r="AK40" s="46" t="n">
-        <v>44.3</v>
+        <v>62.3</v>
       </c>
       <c r="AL40" s="44" t="n"/>
     </row>
@@ -4079,16 +4079,16 @@
         <v>266</v>
       </c>
       <c r="AH41" s="51" t="n">
-        <v>438</v>
+        <v>437.9999999999999</v>
       </c>
       <c r="AI41" s="51" t="n">
-        <v>0.607305936073059</v>
+        <v>0.6073059360730595</v>
       </c>
       <c r="AJ41" s="46" t="n">
-        <v>-5.3</v>
+        <v>-4.5</v>
       </c>
       <c r="AK41" s="46" t="n">
-        <v>35.3</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="AL41" s="44" t="n"/>
     </row>
@@ -4158,13 +4158,13 @@
         <v>1074</v>
       </c>
       <c r="AI42" s="51" t="n">
-        <v>0.339851024208566</v>
+        <v>0.3398510242085661</v>
       </c>
       <c r="AJ42" s="46" t="n">
         <v>-4.4</v>
       </c>
       <c r="AK42" s="46" t="n">
-        <v>88.7</v>
+        <v>101.4</v>
       </c>
     </row>
     <row customFormat="1" customHeight="1" ht="15" r="43" s="46">
@@ -4227,19 +4227,19 @@
         <v>1127</v>
       </c>
       <c r="AG43" s="51" t="n">
-        <v>359</v>
+        <v>359.0000000000001</v>
       </c>
       <c r="AH43" s="51" t="n">
-        <v>596</v>
+        <v>595.9999999999999</v>
       </c>
       <c r="AI43" s="51" t="n">
-        <v>0.602348993288591</v>
+        <v>0.6023489932885908</v>
       </c>
       <c r="AJ43" s="46" t="n">
-        <v>-10.6</v>
+        <v>-10.4</v>
       </c>
       <c r="AK43" s="46" t="n">
-        <v>53.2</v>
+        <v>54.1</v>
       </c>
       <c r="AL43" s="44" t="n"/>
     </row>
@@ -4303,19 +4303,19 @@
         <v>1390</v>
       </c>
       <c r="AG44" s="51" t="n">
-        <v>408</v>
+        <v>408.0000000000001</v>
       </c>
       <c r="AH44" s="51" t="n">
-        <v>796</v>
+        <v>795.9999999999999</v>
       </c>
       <c r="AI44" s="51" t="n">
-        <v>0.512562814070352</v>
+        <v>0.5125628140703519</v>
       </c>
       <c r="AJ44" s="46" t="n">
-        <v>-11.6</v>
+        <v>-11.1</v>
       </c>
       <c r="AK44" s="46" t="n">
-        <v>89.59999999999999</v>
+        <v>91.90000000000001</v>
       </c>
       <c r="AL44" s="44" t="n"/>
     </row>
@@ -4446,19 +4446,19 @@
         <v>801</v>
       </c>
       <c r="AG46" s="51" t="n">
-        <v>317</v>
+        <v>317.0000000000001</v>
       </c>
       <c r="AH46" s="51" t="n">
-        <v>427</v>
+        <v>426.9999999999999</v>
       </c>
       <c r="AI46" s="51" t="n">
-        <v>0.742388758782202</v>
+        <v>0.7423887587822017</v>
       </c>
       <c r="AJ46" s="46" t="n">
-        <v>-11.1</v>
+        <v>-10.8</v>
       </c>
       <c r="AK46" s="46" t="n">
-        <v>57.8</v>
+        <v>58.1</v>
       </c>
       <c r="AL46" s="45" t="n"/>
     </row>
@@ -4528,13 +4528,13 @@
         <v>745</v>
       </c>
       <c r="AI47" s="51" t="n">
-        <v>0.371812080536913</v>
+        <v>0.3718120805369128</v>
       </c>
       <c r="AJ47" s="46" t="n">
-        <v>-3.8</v>
+        <v>-2</v>
       </c>
       <c r="AK47" s="46" t="n">
-        <v>94.59999999999999</v>
+        <v>114.5</v>
       </c>
       <c r="AL47" s="45" t="n"/>
     </row>
@@ -4604,13 +4604,13 @@
         <v>898</v>
       </c>
       <c r="AI48" s="51" t="n">
-        <v>0.385300668151448</v>
+        <v>0.3853006681514476</v>
       </c>
       <c r="AJ48" s="46" t="n">
         <v>-8.699999999999999</v>
       </c>
       <c r="AK48" s="46" t="n">
-        <v>125.1</v>
+        <v>122.1</v>
       </c>
       <c r="AL48" s="45" t="n"/>
     </row>
@@ -4683,10 +4683,10 @@
         <v>-0.288135593220339</v>
       </c>
       <c r="AJ49" s="46" t="n">
-        <v>-5.9</v>
+        <v>-4.4</v>
       </c>
       <c r="AK49" s="46" t="n">
-        <v>64.3</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="AM49" s="27" t="n"/>
       <c r="AN49" s="27" t="n"/>
@@ -4769,16 +4769,16 @@
         <v>312</v>
       </c>
       <c r="AH50" s="46" t="n">
-        <v>830</v>
+        <v>829.9999999999999</v>
       </c>
       <c r="AI50" s="46" t="n">
-        <v>0.375903614457831</v>
+        <v>0.3759036144578314</v>
       </c>
       <c r="AJ50" s="46" t="n">
-        <v>-6.6</v>
+        <v>-6.4</v>
       </c>
       <c r="AK50" s="46" t="n">
-        <v>74.8</v>
+        <v>72.40000000000001</v>
       </c>
       <c r="AL50" s="46" t="n"/>
     </row>
@@ -4848,13 +4848,13 @@
         <v>504</v>
       </c>
       <c r="AI51" s="46" t="n">
-        <v>0.744047619047619</v>
+        <v>0.7440476190476191</v>
       </c>
       <c r="AJ51" s="46" t="n">
         <v>-10.8</v>
       </c>
       <c r="AK51" s="46" t="n">
-        <v>72.2</v>
+        <v>81.40000000000001</v>
       </c>
       <c r="AL51" s="46" t="n"/>
     </row>
@@ -4921,16 +4921,16 @@
         <v>390</v>
       </c>
       <c r="AH52" s="46" t="n">
-        <v>461</v>
+        <v>460.9999999999999</v>
       </c>
       <c r="AI52" s="46" t="n">
-        <v>0.845986984815618</v>
+        <v>0.8459869848156183</v>
       </c>
       <c r="AJ52" s="46" t="n">
-        <v>-9.6</v>
+        <v>-8.1</v>
       </c>
       <c r="AK52" s="46" t="n">
-        <v>73.59999999999999</v>
+        <v>92.7</v>
       </c>
       <c r="AL52" s="46" t="n"/>
     </row>

</xml_diff>

<commit_message>
Synced all curves with the valves times+peak plt fixed(include positive)
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1060,55 +1060,55 @@
         <v>382</v>
       </c>
       <c r="U3" s="44" t="n">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="V3" s="44" t="n">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="W3" s="44" t="n">
-        <v>1170</v>
+        <v>1147</v>
       </c>
       <c r="X3" s="45" t="n">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="Y3" s="45" t="n">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="Z3" s="44" t="n">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="AA3" s="44" t="n">
-        <v>581</v>
+        <v>571</v>
       </c>
       <c r="AB3" s="44" t="n">
-        <v>652</v>
+        <v>640</v>
       </c>
       <c r="AC3" s="44" t="n">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="AD3" s="44" t="n">
-        <v>1170</v>
+        <v>1147</v>
       </c>
       <c r="AE3" s="44" t="n">
-        <v>1246</v>
+        <v>1440</v>
       </c>
       <c r="AF3" s="44" t="n">
-        <v>1294</v>
+        <v>1480</v>
       </c>
       <c r="AG3" s="45" t="n">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="AH3" s="45" t="n">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="AI3" s="46" t="n">
-        <v>0.4143518518518519</v>
+        <v>0.4192799070847851</v>
       </c>
       <c r="AJ3" s="46" t="n">
         <v>-17.9</v>
       </c>
       <c r="AK3" s="46" t="n">
-        <v>38.4</v>
+        <v>36.6</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="4" s="29">
@@ -1147,16 +1147,16 @@
         <v>95</v>
       </c>
       <c r="Y4" s="45" t="n">
-        <v>236</v>
+        <v>160</v>
       </c>
       <c r="Z4" s="46" t="n">
-        <v>312</v>
+        <v>240</v>
       </c>
       <c r="AA4" s="46" t="n">
-        <v>614</v>
+        <v>539</v>
       </c>
       <c r="AB4" s="46" t="n">
-        <v>795</v>
+        <v>720</v>
       </c>
       <c r="AC4" s="46" t="n">
         <v>1066</v>
@@ -1165,19 +1165,19 @@
         <v>968</v>
       </c>
       <c r="AE4" s="46" t="n">
-        <v>1183</v>
+        <v>1290</v>
       </c>
       <c r="AF4" s="46" t="n">
-        <v>1259</v>
+        <v>1370</v>
       </c>
       <c r="AG4" s="45" t="n">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AH4" s="45" t="n">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="AI4" s="46" t="n">
-        <v>0.5006622516556292</v>
+        <v>0.5026525198938993</v>
       </c>
       <c r="AJ4" s="46" t="n">
         <v>-6.7</v>
@@ -1679,16 +1679,16 @@
         <v>52</v>
       </c>
       <c r="Y10" s="45" t="n">
-        <v>808</v>
+        <v>840</v>
       </c>
       <c r="Z10" s="46" t="n">
-        <v>225</v>
+        <v>260</v>
       </c>
       <c r="AA10" s="46" t="n">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="AB10" s="46" t="n">
-        <v>517</v>
+        <v>550</v>
       </c>
       <c r="AC10" s="46" t="n">
         <v>758</v>
@@ -1697,25 +1697,25 @@
         <v>694</v>
       </c>
       <c r="AE10" s="46" t="n">
-        <v>1491</v>
+        <v>1660</v>
       </c>
       <c r="AF10" s="46" t="n">
-        <v>908</v>
+        <v>1080</v>
       </c>
       <c r="AG10" s="45" t="n">
-        <v>-388.0000000000001</v>
+        <v>-384.9999999999999</v>
       </c>
       <c r="AH10" s="45" t="n">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="AI10" s="46" t="n">
-        <v>-0.3219917012448133</v>
+        <v>-0.3202995008319467</v>
       </c>
       <c r="AJ10" s="46" t="n">
         <v>-2.5</v>
       </c>
       <c r="AK10" s="46" t="n">
-        <v>123.7</v>
+        <v>137.5</v>
       </c>
       <c r="AL10" s="44" t="n"/>
     </row>
@@ -2077,10 +2077,10 @@
         <v>1254</v>
       </c>
       <c r="AE15" s="46" t="n">
-        <v>1290</v>
+        <v>1503</v>
       </c>
       <c r="AF15" s="46" t="n">
-        <v>1373</v>
+        <v>1586</v>
       </c>
       <c r="AG15" s="45" t="n">
         <v>389</v>
@@ -2095,7 +2095,7 @@
         <v>-7.3</v>
       </c>
       <c r="AK15" s="46" t="n">
-        <v>103.2</v>
+        <v>39.7</v>
       </c>
       <c r="AL15" s="44" t="n"/>
     </row>
@@ -2667,16 +2667,16 @@
         <v>103</v>
       </c>
       <c r="Y23" s="45" t="n">
-        <v>996</v>
+        <v>1003</v>
       </c>
       <c r="Z23" s="46" t="n">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="AA23" s="46" t="n">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="AB23" s="46" t="n">
-        <v>599</v>
+        <v>606</v>
       </c>
       <c r="AC23" s="46" t="n">
         <v>1034</v>
@@ -2685,13 +2685,13 @@
         <v>1167</v>
       </c>
       <c r="AE23" s="46" t="n">
-        <v>2037</v>
+        <v>2244</v>
       </c>
       <c r="AF23" s="46" t="n">
-        <v>1315</v>
+        <v>1522</v>
       </c>
       <c r="AG23" s="45" t="n">
-        <v>-441.9999999999999</v>
+        <v>-442.0000000000001</v>
       </c>
       <c r="AH23" s="45" t="n">
         <v>1683</v>
@@ -2703,7 +2703,7 @@
         <v>-16.7</v>
       </c>
       <c r="AK23" s="46" t="n">
-        <v>99.59999999999999</v>
+        <v>57.5</v>
       </c>
       <c r="AL23" s="46" t="n"/>
     </row>

</xml_diff>

<commit_message>
Created a function that shows the segments' name
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -2667,16 +2667,16 @@
         <v>103</v>
       </c>
       <c r="Y23" s="45" t="n">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="Z23" s="46" t="n">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AA23" s="46" t="n">
         <v>561</v>
       </c>
       <c r="AB23" s="46" t="n">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="AC23" s="46" t="n">
         <v>1034</v>
@@ -2685,19 +2685,19 @@
         <v>1167</v>
       </c>
       <c r="AE23" s="46" t="n">
-        <v>2244</v>
+        <v>2240</v>
       </c>
       <c r="AF23" s="46" t="n">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="AG23" s="45" t="n">
-        <v>-442.0000000000001</v>
+        <v>-438.9999999999999</v>
       </c>
       <c r="AH23" s="45" t="n">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="AI23" s="46" t="n">
-        <v>-0.2626262626262626</v>
+        <v>-0.2613095238095238</v>
       </c>
       <c r="AJ23" s="46" t="n">
         <v>-16.7</v>

</xml_diff>

<commit_message>
Last adjustments before v2 - new function to clear the terminal
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -1066,16 +1066,16 @@
         <v>382</v>
       </c>
       <c r="U3" s="45" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="V3" s="45" t="n">
-        <v>1030</v>
+        <v>1016</v>
       </c>
       <c r="W3" s="45" t="n">
-        <v>1190</v>
+        <v>1195</v>
       </c>
       <c r="X3" s="46" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Y3" s="46" t="n">
         <v>210</v>
@@ -1090,10 +1090,10 @@
         <v>640</v>
       </c>
       <c r="AC3" s="45" t="n">
-        <v>1030</v>
+        <v>1016</v>
       </c>
       <c r="AD3" s="45" t="n">
-        <v>1190</v>
+        <v>1195</v>
       </c>
       <c r="AE3" s="45" t="n">
         <v>1440</v>
@@ -1141,16 +1141,16 @@
         <v>428</v>
       </c>
       <c r="U4" s="45" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="V4" s="45" t="n">
-        <v>985</v>
+        <v>993</v>
       </c>
       <c r="W4" s="45" t="n">
         <v>1114</v>
       </c>
       <c r="X4" s="46" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="Y4" s="46" t="n">
         <v>160</v>
@@ -1165,7 +1165,7 @@
         <v>720</v>
       </c>
       <c r="AC4" s="47" t="n">
-        <v>985</v>
+        <v>993</v>
       </c>
       <c r="AD4" s="47" t="n">
         <v>1114</v>
@@ -1186,10 +1186,10 @@
         <v>0.5026525198938993</v>
       </c>
       <c r="AJ4" s="47" t="n">
-        <v>-6.7</v>
+        <v>-7.5</v>
       </c>
       <c r="AK4" s="47" t="n">
-        <v>118.7</v>
+        <v>151.8</v>
       </c>
       <c r="AL4" s="28" t="n">
         <v>1</v>
@@ -1288,16 +1288,16 @@
         <v>441</v>
       </c>
       <c r="U5" s="45" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="V5" s="45" t="n">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="W5" s="45" t="n">
-        <v>1176</v>
+        <v>1181</v>
       </c>
       <c r="X5" s="46" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="Y5" s="46" t="n">
         <v>280</v>
@@ -1312,10 +1312,10 @@
         <v>770</v>
       </c>
       <c r="AC5" s="47" t="n">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="AD5" s="47" t="n">
-        <v>1176</v>
+        <v>1181</v>
       </c>
       <c r="AE5" s="47" t="n">
         <v>1490</v>
@@ -1327,16 +1327,16 @@
         <v>405</v>
       </c>
       <c r="AH5" s="46" t="n">
-        <v>807</v>
+        <v>806.9999999999999</v>
       </c>
       <c r="AI5" s="47" t="n">
-        <v>0.5018587360594799</v>
+        <v>0.5018587360594796</v>
       </c>
       <c r="AJ5" s="47" t="n">
-        <v>-10.6</v>
+        <v>-11.6</v>
       </c>
       <c r="AK5" s="47" t="n">
-        <v>101.9</v>
+        <v>77.40000000000001</v>
       </c>
       <c r="AL5" s="45" t="n"/>
     </row>
@@ -1518,16 +1518,16 @@
         <v>460</v>
       </c>
       <c r="U8" s="45" t="n">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="V8" s="45" t="n">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="W8" s="45" t="n">
-        <v>909</v>
+        <v>1120</v>
       </c>
       <c r="X8" s="46" t="n">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="Y8" s="46" t="n">
         <v>1090</v>
@@ -1542,10 +1542,10 @@
         <v>680</v>
       </c>
       <c r="AC8" s="47" t="n">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="AD8" s="47" t="n">
-        <v>909</v>
+        <v>1120</v>
       </c>
       <c r="AE8" s="47" t="n">
         <v>2230</v>
@@ -1554,13 +1554,13 @@
         <v>1400</v>
       </c>
       <c r="AG8" s="46" t="n">
-        <v>-439</v>
+        <v>-439.0000000000001</v>
       </c>
       <c r="AH8" s="46" t="n">
         <v>1575</v>
       </c>
       <c r="AI8" s="47" t="n">
-        <v>-0.278730158730159</v>
+        <v>-0.2787301587301588</v>
       </c>
       <c r="AJ8" s="47" t="n">
         <v>-13.6</v>
@@ -1597,16 +1597,16 @@
         <v>395</v>
       </c>
       <c r="U9" s="45" t="n">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="V9" s="45" t="n">
-        <v>930</v>
+        <v>820</v>
       </c>
       <c r="W9" s="45" t="n">
-        <v>804</v>
+        <v>1001</v>
       </c>
       <c r="X9" s="46" t="n">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="Y9" s="46" t="n">
         <v>1060</v>
@@ -1621,10 +1621,10 @@
         <v>650</v>
       </c>
       <c r="AC9" s="47" t="n">
-        <v>930</v>
+        <v>820</v>
       </c>
       <c r="AD9" s="47" t="n">
-        <v>804</v>
+        <v>1001</v>
       </c>
       <c r="AE9" s="47" t="n">
         <v>2090</v>
@@ -1633,13 +1633,13 @@
         <v>1260</v>
       </c>
       <c r="AG9" s="46" t="n">
-        <v>-490</v>
+        <v>-490.0000000000001</v>
       </c>
       <c r="AH9" s="46" t="n">
         <v>1517</v>
       </c>
       <c r="AI9" s="47" t="n">
-        <v>-0.32300593276203</v>
+        <v>-0.3230059327620304</v>
       </c>
       <c r="AJ9" s="47" t="n">
         <v>-18.3</v>
@@ -1673,16 +1673,16 @@
         <v>286</v>
       </c>
       <c r="U10" s="45" t="n">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="V10" s="45" t="n">
-        <v>758</v>
+        <v>688</v>
       </c>
       <c r="W10" s="45" t="n">
-        <v>694</v>
+        <v>790</v>
       </c>
       <c r="X10" s="46" t="n">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="Y10" s="46" t="n">
         <v>840</v>
@@ -1697,10 +1697,10 @@
         <v>550</v>
       </c>
       <c r="AC10" s="47" t="n">
-        <v>758</v>
+        <v>688</v>
       </c>
       <c r="AD10" s="47" t="n">
-        <v>694</v>
+        <v>790</v>
       </c>
       <c r="AE10" s="47" t="n">
         <v>1660</v>
@@ -1709,19 +1709,19 @@
         <v>1080</v>
       </c>
       <c r="AG10" s="46" t="n">
-        <v>-385</v>
+        <v>-384.9999999999999</v>
       </c>
       <c r="AH10" s="46" t="n">
         <v>1202</v>
       </c>
       <c r="AI10" s="47" t="n">
-        <v>-0.320299500831947</v>
+        <v>-0.3202995008319467</v>
       </c>
       <c r="AJ10" s="47" t="n">
-        <v>-2.5</v>
+        <v>-4.6</v>
       </c>
       <c r="AK10" s="47" t="n">
-        <v>137.5</v>
+        <v>96.2</v>
       </c>
       <c r="AL10" s="45" t="n"/>
     </row>
@@ -1749,16 +1749,16 @@
         <v>311</v>
       </c>
       <c r="U11" s="45" t="n">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="V11" s="45" t="n">
-        <v>752</v>
+        <v>703</v>
       </c>
       <c r="W11" s="45" t="n">
-        <v>690</v>
+        <v>784</v>
       </c>
       <c r="X11" s="46" t="n">
-        <v>25</v>
+        <v>101</v>
       </c>
       <c r="Y11" s="46" t="n">
         <v>800</v>
@@ -1773,10 +1773,10 @@
         <v>520</v>
       </c>
       <c r="AC11" s="47" t="n">
-        <v>752</v>
+        <v>703</v>
       </c>
       <c r="AD11" s="47" t="n">
-        <v>690</v>
+        <v>784</v>
       </c>
       <c r="AE11" s="47" t="n">
         <v>1610</v>
@@ -1785,13 +1785,13 @@
         <v>980</v>
       </c>
       <c r="AG11" s="46" t="n">
-        <v>-359</v>
+        <v>-359.0000000000001</v>
       </c>
       <c r="AH11" s="46" t="n">
         <v>1170</v>
       </c>
       <c r="AI11" s="47" t="n">
-        <v>-0.306837606837607</v>
+        <v>-0.3068376068376069</v>
       </c>
       <c r="AJ11" s="47" t="n">
         <v>-21.6</v>
@@ -1825,16 +1825,16 @@
         <v>375</v>
       </c>
       <c r="U12" s="45" t="n">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="V12" s="45" t="n">
-        <v>1060</v>
+        <v>951</v>
       </c>
       <c r="W12" s="45" t="n">
-        <v>937</v>
+        <v>1106</v>
       </c>
       <c r="X12" s="46" t="n">
-        <v>74</v>
+        <v>144</v>
       </c>
       <c r="Y12" s="46" t="n">
         <v>210</v>
@@ -1849,10 +1849,10 @@
         <v>650</v>
       </c>
       <c r="AC12" s="47" t="n">
-        <v>1060</v>
+        <v>951</v>
       </c>
       <c r="AD12" s="47" t="n">
-        <v>937</v>
+        <v>1106</v>
       </c>
       <c r="AE12" s="47" t="n">
         <v>1330</v>
@@ -1861,13 +1861,13 @@
         <v>1360</v>
       </c>
       <c r="AG12" s="46" t="n">
-        <v>342</v>
+        <v>342.0000000000001</v>
       </c>
       <c r="AH12" s="46" t="n">
-        <v>779</v>
+        <v>778.9999999999999</v>
       </c>
       <c r="AI12" s="47" t="n">
-        <v>0.439024390243903</v>
+        <v>0.4390243902439026</v>
       </c>
       <c r="AJ12" s="47" t="n">
         <v>-16.3</v>
@@ -1901,16 +1901,16 @@
         <v>294</v>
       </c>
       <c r="U13" s="45" t="n">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="V13" s="45" t="n">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="W13" s="45" t="n">
-        <v>682</v>
+        <v>885</v>
       </c>
       <c r="X13" s="46" t="n">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="Y13" s="46" t="n">
         <v>900</v>
@@ -1925,10 +1925,10 @@
         <v>550</v>
       </c>
       <c r="AC13" s="47" t="n">
-        <v>779</v>
+        <v>771</v>
       </c>
       <c r="AD13" s="47" t="n">
-        <v>682</v>
+        <v>885</v>
       </c>
       <c r="AE13" s="47" t="n">
         <v>1800</v>
@@ -1943,13 +1943,13 @@
         <v>1364</v>
       </c>
       <c r="AI13" s="47" t="n">
-        <v>-0.342375366568915</v>
+        <v>-0.3423753665689149</v>
       </c>
       <c r="AJ13" s="47" t="n">
-        <v>-11.2</v>
+        <v>-11.6</v>
       </c>
       <c r="AK13" s="47" t="n">
-        <v>59.4</v>
+        <v>51.2</v>
       </c>
       <c r="AL13" s="45" t="n"/>
     </row>
@@ -2053,16 +2053,16 @@
         <v>399</v>
       </c>
       <c r="U15" s="45" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="V15" s="45" t="n">
-        <v>1088</v>
+        <v>1167</v>
       </c>
       <c r="W15" s="45" t="n">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="X15" s="46" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Y15" s="46" t="n">
         <v>220</v>
@@ -2077,10 +2077,10 @@
         <v>700</v>
       </c>
       <c r="AC15" s="47" t="n">
-        <v>1088</v>
+        <v>1167</v>
       </c>
       <c r="AD15" s="47" t="n">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="AE15" s="47" t="n">
         <v>1500</v>
@@ -2095,7 +2095,7 @@
         <v>888</v>
       </c>
       <c r="AI15" s="47" t="n">
-        <v>0.441441441441441</v>
+        <v>0.4414414414414414</v>
       </c>
       <c r="AJ15" s="47" t="n">
         <v>-7.3</v>
@@ -2129,16 +2129,16 @@
         <v>374</v>
       </c>
       <c r="U16" s="47" t="n">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="V16" s="47" t="n">
-        <v>888</v>
+        <v>771</v>
       </c>
       <c r="W16" s="47" t="n">
-        <v>767</v>
+        <v>937</v>
       </c>
       <c r="X16" s="46" t="n">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="Y16" s="46" t="n">
         <v>170</v>
@@ -2153,10 +2153,10 @@
         <v>610</v>
       </c>
       <c r="AC16" s="47" t="n">
-        <v>888</v>
+        <v>771</v>
       </c>
       <c r="AD16" s="47" t="n">
-        <v>767</v>
+        <v>937</v>
       </c>
       <c r="AE16" s="47" t="n">
         <v>1130</v>
@@ -2171,7 +2171,7 @@
         <v>590</v>
       </c>
       <c r="AI16" s="47" t="n">
-        <v>0.622033898305085</v>
+        <v>0.6220338983050848</v>
       </c>
       <c r="AJ16" s="47" t="n">
         <v>-17.4</v>
@@ -2205,16 +2205,16 @@
         <v>384</v>
       </c>
       <c r="U17" s="47" t="n">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="V17" s="47" t="n">
-        <v>939</v>
+        <v>828</v>
       </c>
       <c r="W17" s="47" t="n">
-        <v>810</v>
+        <v>1022</v>
       </c>
       <c r="X17" s="46" t="n">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="Y17" s="46" t="n">
         <v>1060</v>
@@ -2229,10 +2229,10 @@
         <v>650</v>
       </c>
       <c r="AC17" s="47" t="n">
-        <v>939</v>
+        <v>828</v>
       </c>
       <c r="AD17" s="47" t="n">
-        <v>810</v>
+        <v>1022</v>
       </c>
       <c r="AE17" s="47" t="n">
         <v>2120</v>
@@ -2247,7 +2247,7 @@
         <v>1570</v>
       </c>
       <c r="AI17" s="47" t="n">
-        <v>-0.329299363057325</v>
+        <v>-0.3292993630573249</v>
       </c>
       <c r="AJ17" s="47" t="n">
         <v>-20.2</v>
@@ -2281,16 +2281,16 @@
         <v>326</v>
       </c>
       <c r="U18" s="47" t="n">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="V18" s="47" t="n">
-        <v>925</v>
+        <v>896</v>
       </c>
       <c r="W18" s="47" t="n">
-        <v>835</v>
+        <v>1001</v>
       </c>
       <c r="X18" s="46" t="n">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="Y18" s="46" t="n">
         <v>1060</v>
@@ -2305,10 +2305,10 @@
         <v>580</v>
       </c>
       <c r="AC18" s="47" t="n">
-        <v>925</v>
+        <v>896</v>
       </c>
       <c r="AD18" s="47" t="n">
-        <v>835</v>
+        <v>1001</v>
       </c>
       <c r="AE18" s="47" t="n">
         <v>2090</v>
@@ -2323,7 +2323,7 @@
         <v>1572</v>
       </c>
       <c r="AI18" s="47" t="n">
-        <v>-0.348600508905852</v>
+        <v>-0.3486005089058524</v>
       </c>
       <c r="AJ18" s="47" t="n">
         <v>-19.6</v>
@@ -2357,16 +2357,16 @@
         <v>385</v>
       </c>
       <c r="U19" s="47" t="n">
-        <v>116</v>
+        <v>186</v>
       </c>
       <c r="V19" s="47" t="n">
-        <v>1216</v>
+        <v>1076</v>
       </c>
       <c r="W19" s="47" t="n">
-        <v>1110</v>
+        <v>1292</v>
       </c>
       <c r="X19" s="46" t="n">
-        <v>116</v>
+        <v>186</v>
       </c>
       <c r="Y19" s="46" t="n">
         <v>220</v>
@@ -2381,10 +2381,10 @@
         <v>730</v>
       </c>
       <c r="AC19" s="47" t="n">
-        <v>1216</v>
+        <v>1076</v>
       </c>
       <c r="AD19" s="47" t="n">
-        <v>1110</v>
+        <v>1292</v>
       </c>
       <c r="AE19" s="47" t="n">
         <v>1540</v>
@@ -2396,10 +2396,10 @@
         <v>376</v>
       </c>
       <c r="AH19" s="46" t="n">
-        <v>944</v>
+        <v>944.0000000000001</v>
       </c>
       <c r="AI19" s="47" t="n">
-        <v>0.398305084745763</v>
+        <v>0.3983050847457627</v>
       </c>
       <c r="AJ19" s="47" t="n">
         <v>-15.1</v>
@@ -2661,16 +2661,16 @@
         <v>354</v>
       </c>
       <c r="U23" s="47" t="n">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="V23" s="47" t="n">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="W23" s="47" t="n">
-        <v>1167</v>
+        <v>1217</v>
       </c>
       <c r="X23" s="46" t="n">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="Y23" s="46" t="n">
         <v>1000</v>
@@ -2685,10 +2685,10 @@
         <v>610</v>
       </c>
       <c r="AC23" s="47" t="n">
-        <v>1034</v>
+        <v>1039</v>
       </c>
       <c r="AD23" s="47" t="n">
-        <v>1167</v>
+        <v>1217</v>
       </c>
       <c r="AE23" s="47" t="n">
         <v>2240</v>
@@ -2697,13 +2697,13 @@
         <v>1520</v>
       </c>
       <c r="AG23" s="46" t="n">
-        <v>-439</v>
+        <v>-438.9999999999999</v>
       </c>
       <c r="AH23" s="46" t="n">
         <v>1680</v>
       </c>
       <c r="AI23" s="47" t="n">
-        <v>-0.261309523809524</v>
+        <v>-0.2613095238095238</v>
       </c>
       <c r="AJ23" s="47" t="n">
         <v>-16.7</v>
@@ -3345,16 +3345,16 @@
         <v>385</v>
       </c>
       <c r="U32" s="47" t="n">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="V32" s="47" t="n">
-        <v>1255</v>
+        <v>1160</v>
       </c>
       <c r="W32" s="47" t="n">
-        <v>1125</v>
+        <v>1304</v>
       </c>
       <c r="X32" s="47" t="n">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="Y32" s="47" t="n">
         <v>220</v>
@@ -3369,10 +3369,10 @@
         <v>680</v>
       </c>
       <c r="AC32" s="47" t="n">
-        <v>1255</v>
+        <v>1160</v>
       </c>
       <c r="AD32" s="47" t="n">
-        <v>1125</v>
+        <v>1304</v>
       </c>
       <c r="AE32" s="47" t="n">
         <v>1550</v>
@@ -3384,16 +3384,16 @@
         <v>378</v>
       </c>
       <c r="AH32" s="47" t="n">
-        <v>950</v>
+        <v>950.0000000000001</v>
       </c>
       <c r="AI32" s="47" t="n">
-        <v>0.397894736842105</v>
+        <v>0.3978947368421052</v>
       </c>
       <c r="AJ32" s="47" t="n">
-        <v>-17</v>
+        <v>-16.4</v>
       </c>
       <c r="AK32" s="47" t="n">
-        <v>28.1</v>
+        <v>33.7</v>
       </c>
       <c r="AL32" s="46" t="n"/>
       <c r="AM32" s="47" t="n"/>

</xml_diff>

<commit_message>
Started to optimize how the files are read
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -627,13 +627,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BI55"/>
+  <dimension ref="A1:BI56"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO2" activeCellId="0" sqref="AO2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A26" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.8671875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="28.14" customWidth="1" style="27" min="1" max="1"/>
     <col width="60" customWidth="1" style="27" min="2" max="2"/>
@@ -696,7 +696,7 @@
     <col width="14.54" customWidth="1" style="27" min="59" max="59"/>
     <col width="12.61" customWidth="1" style="27" min="60" max="60"/>
     <col width="12.83" customWidth="1" style="27" min="61" max="61"/>
-    <col width="9.85" customWidth="1" style="27" min="62" max="1025"/>
+    <col width="9.85" customWidth="1" style="27" min="62" max="1024"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.5" customHeight="1" s="29">
@@ -1108,7 +1108,7 @@
         <v>861</v>
       </c>
       <c r="AI3" s="47" t="n">
-        <v>0.4192799070847851</v>
+        <v>0.419279907084785</v>
       </c>
       <c r="AJ3" s="47" t="n">
         <v>-17.9</v>
@@ -1183,7 +1183,7 @@
         <v>754</v>
       </c>
       <c r="AI4" s="47" t="n">
-        <v>0.5026525198938993</v>
+        <v>0.502652519893899</v>
       </c>
       <c r="AJ4" s="47" t="n">
         <v>-7.5</v>
@@ -1327,10 +1327,10 @@
         <v>405</v>
       </c>
       <c r="AH5" s="46" t="n">
-        <v>806.9999999999999</v>
+        <v>807</v>
       </c>
       <c r="AI5" s="47" t="n">
-        <v>0.5018587360594796</v>
+        <v>0.5018587360594799</v>
       </c>
       <c r="AJ5" s="47" t="n">
         <v>-11.6</v>
@@ -1554,13 +1554,13 @@
         <v>1400</v>
       </c>
       <c r="AG8" s="46" t="n">
-        <v>-439.0000000000001</v>
+        <v>-439</v>
       </c>
       <c r="AH8" s="46" t="n">
         <v>1575</v>
       </c>
       <c r="AI8" s="47" t="n">
-        <v>-0.2787301587301588</v>
+        <v>-0.278730158730159</v>
       </c>
       <c r="AJ8" s="47" t="n">
         <v>-13.6</v>
@@ -1633,13 +1633,13 @@
         <v>1260</v>
       </c>
       <c r="AG9" s="46" t="n">
-        <v>-490.0000000000001</v>
+        <v>-490</v>
       </c>
       <c r="AH9" s="46" t="n">
         <v>1517</v>
       </c>
       <c r="AI9" s="47" t="n">
-        <v>-0.3230059327620304</v>
+        <v>-0.32300593276203</v>
       </c>
       <c r="AJ9" s="47" t="n">
         <v>-18.3</v>
@@ -1709,13 +1709,13 @@
         <v>1080</v>
       </c>
       <c r="AG10" s="46" t="n">
-        <v>-384.9999999999999</v>
+        <v>-385</v>
       </c>
       <c r="AH10" s="46" t="n">
         <v>1202</v>
       </c>
       <c r="AI10" s="47" t="n">
-        <v>-0.3202995008319467</v>
+        <v>-0.320299500831947</v>
       </c>
       <c r="AJ10" s="47" t="n">
         <v>-4.6</v>
@@ -1785,13 +1785,13 @@
         <v>980</v>
       </c>
       <c r="AG11" s="46" t="n">
-        <v>-359.0000000000001</v>
+        <v>-359</v>
       </c>
       <c r="AH11" s="46" t="n">
         <v>1170</v>
       </c>
       <c r="AI11" s="47" t="n">
-        <v>-0.3068376068376069</v>
+        <v>-0.306837606837607</v>
       </c>
       <c r="AJ11" s="47" t="n">
         <v>-21.6</v>
@@ -1861,13 +1861,13 @@
         <v>1360</v>
       </c>
       <c r="AG12" s="46" t="n">
-        <v>342.0000000000001</v>
+        <v>342</v>
       </c>
       <c r="AH12" s="46" t="n">
-        <v>778.9999999999999</v>
+        <v>779</v>
       </c>
       <c r="AI12" s="47" t="n">
-        <v>0.4390243902439026</v>
+        <v>0.439024390243903</v>
       </c>
       <c r="AJ12" s="47" t="n">
         <v>-16.3</v>
@@ -1943,7 +1943,7 @@
         <v>1364</v>
       </c>
       <c r="AI13" s="47" t="n">
-        <v>-0.3423753665689149</v>
+        <v>-0.342375366568915</v>
       </c>
       <c r="AJ13" s="47" t="n">
         <v>-11.6</v>
@@ -2095,7 +2095,7 @@
         <v>888</v>
       </c>
       <c r="AI15" s="47" t="n">
-        <v>0.4414414414414414</v>
+        <v>0.441441441441441</v>
       </c>
       <c r="AJ15" s="47" t="n">
         <v>-7.3</v>
@@ -2171,7 +2171,7 @@
         <v>590</v>
       </c>
       <c r="AI16" s="47" t="n">
-        <v>0.6220338983050848</v>
+        <v>0.622033898305085</v>
       </c>
       <c r="AJ16" s="47" t="n">
         <v>-17.4</v>
@@ -2247,7 +2247,7 @@
         <v>1570</v>
       </c>
       <c r="AI17" s="47" t="n">
-        <v>-0.3292993630573249</v>
+        <v>-0.329299363057325</v>
       </c>
       <c r="AJ17" s="47" t="n">
         <v>-20.2</v>
@@ -2323,7 +2323,7 @@
         <v>1572</v>
       </c>
       <c r="AI18" s="47" t="n">
-        <v>-0.3486005089058524</v>
+        <v>-0.348600508905852</v>
       </c>
       <c r="AJ18" s="47" t="n">
         <v>-19.6</v>
@@ -2396,10 +2396,10 @@
         <v>376</v>
       </c>
       <c r="AH19" s="46" t="n">
-        <v>944.0000000000001</v>
+        <v>944</v>
       </c>
       <c r="AI19" s="47" t="n">
-        <v>0.3983050847457627</v>
+        <v>0.398305084745763</v>
       </c>
       <c r="AJ19" s="47" t="n">
         <v>-15.1</v>
@@ -2697,13 +2697,13 @@
         <v>1520</v>
       </c>
       <c r="AG23" s="46" t="n">
-        <v>-438.9999999999999</v>
+        <v>-439</v>
       </c>
       <c r="AH23" s="46" t="n">
         <v>1680</v>
       </c>
       <c r="AI23" s="47" t="n">
-        <v>-0.2613095238095238</v>
+        <v>-0.261309523809524</v>
       </c>
       <c r="AJ23" s="47" t="n">
         <v>-16.7</v>
@@ -3384,10 +3384,10 @@
         <v>378</v>
       </c>
       <c r="AH32" s="47" t="n">
-        <v>950.0000000000001</v>
+        <v>950</v>
       </c>
       <c r="AI32" s="47" t="n">
-        <v>0.3978947368421052</v>
+        <v>0.397894736842105</v>
       </c>
       <c r="AJ32" s="47" t="n">
         <v>-16.4</v>
@@ -4976,7 +4976,81 @@
         </is>
       </c>
     </row>
-    <row r="56" ht="15" customHeight="1" s="29"/>
+    <row r="56" ht="15" customHeight="1" s="29">
+      <c r="A56" s="45" t="inlineStr">
+        <is>
+          <t>AristotelesTest</t>
+        </is>
+      </c>
+      <c r="B56" s="45" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="Q56" s="45" t="n">
+        <v>453</v>
+      </c>
+      <c r="R56" s="45" t="n">
+        <v>24</v>
+      </c>
+      <c r="S56" s="45" t="n">
+        <v>72</v>
+      </c>
+      <c r="T56" s="45" t="n">
+        <v>382</v>
+      </c>
+      <c r="U56" s="45" t="n">
+        <v>160</v>
+      </c>
+      <c r="V56" s="45" t="n">
+        <v>1016</v>
+      </c>
+      <c r="W56" s="45" t="n">
+        <v>1195</v>
+      </c>
+      <c r="X56" s="46" t="n">
+        <v>160</v>
+      </c>
+      <c r="Y56" s="46" t="n">
+        <v>210</v>
+      </c>
+      <c r="Z56" s="45" t="n">
+        <v>260</v>
+      </c>
+      <c r="AA56" s="45" t="n">
+        <v>571</v>
+      </c>
+      <c r="AB56" s="45" t="n">
+        <v>640</v>
+      </c>
+      <c r="AC56" s="45" t="n">
+        <v>1016</v>
+      </c>
+      <c r="AD56" s="45" t="n">
+        <v>1195</v>
+      </c>
+      <c r="AE56" s="45" t="n">
+        <v>1440</v>
+      </c>
+      <c r="AF56" s="45" t="n">
+        <v>1480</v>
+      </c>
+      <c r="AG56" s="46" t="n">
+        <v>361</v>
+      </c>
+      <c r="AH56" s="46" t="n">
+        <v>861</v>
+      </c>
+      <c r="AI56" s="47" t="n">
+        <v>0.4192799070847851</v>
+      </c>
+      <c r="AJ56" s="47" t="n">
+        <v>-17.9</v>
+      </c>
+      <c r="AK56" s="47" t="n">
+        <v>36.6</v>
+      </c>
+    </row>
     <row r="57" ht="15" customHeight="1" s="29"/>
     <row r="58" ht="15" customHeight="1" s="29"/>
     <row r="59" ht="15" customHeight="1" s="29"/>

</xml_diff>

<commit_message>
Added new patient for LAPhases, corrected openfcn
</commit_message>
<xml_diff>
--- a/Patients_DB.xlsx
+++ b/Patients_DB.xlsx
@@ -627,10 +627,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:BI56"/>
+  <dimension ref="A1:BI57"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A26" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A16" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.8671875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
@@ -1108,7 +1108,7 @@
         <v>861</v>
       </c>
       <c r="AI3" s="47" t="n">
-        <v>0.4192799070847851</v>
+        <v>0.419279907084785</v>
       </c>
       <c r="AJ3" s="47" t="n">
         <v>-17.9</v>
@@ -4979,79 +4979,115 @@
     <row r="56" ht="15" customHeight="1" s="29">
       <c r="A56" s="45" t="inlineStr">
         <is>
-          <t>AristotelesTest</t>
+          <t>LBBB_Teste</t>
         </is>
       </c>
       <c r="B56" s="45" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>LBBB</t>
         </is>
       </c>
       <c r="Q56" s="45" t="n">
-        <v>453</v>
+        <v>581</v>
       </c>
       <c r="R56" s="45" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="S56" s="45" t="n">
-        <v>72</v>
+        <v>176</v>
       </c>
       <c r="T56" s="45" t="n">
-        <v>382</v>
-      </c>
-      <c r="U56" s="45" t="n">
-        <v>160</v>
-      </c>
-      <c r="V56" s="45" t="n">
-        <v>1016</v>
-      </c>
-      <c r="W56" s="45" t="n">
-        <v>1195</v>
-      </c>
-      <c r="X56" s="46" t="n">
-        <v>160</v>
-      </c>
-      <c r="Y56" s="46" t="n">
-        <v>210</v>
-      </c>
-      <c r="Z56" s="45" t="n">
-        <v>260</v>
-      </c>
-      <c r="AA56" s="45" t="n">
-        <v>571</v>
-      </c>
-      <c r="AB56" s="45" t="n">
-        <v>640</v>
-      </c>
-      <c r="AC56" s="45" t="n">
-        <v>1016</v>
-      </c>
-      <c r="AD56" s="45" t="n">
-        <v>1195</v>
-      </c>
-      <c r="AE56" s="45" t="n">
-        <v>1440</v>
-      </c>
-      <c r="AF56" s="45" t="n">
-        <v>1480</v>
-      </c>
-      <c r="AG56" s="46" t="n">
-        <v>361</v>
-      </c>
-      <c r="AH56" s="46" t="n">
-        <v>861</v>
-      </c>
-      <c r="AI56" s="47" t="n">
-        <v>0.4192799070847851</v>
-      </c>
-      <c r="AJ56" s="47" t="n">
-        <v>-17.9</v>
-      </c>
-      <c r="AK56" s="47" t="n">
-        <v>36.6</v>
-      </c>
-    </row>
-    <row r="57" ht="15" customHeight="1" s="29"/>
+        <v>467</v>
+      </c>
+      <c r="U56" s="45" t="n"/>
+      <c r="V56" s="45" t="n"/>
+      <c r="W56" s="45" t="n"/>
+      <c r="X56" s="46" t="n"/>
+      <c r="Y56" s="46" t="n"/>
+      <c r="Z56" s="45" t="n"/>
+      <c r="AA56" s="45" t="n"/>
+      <c r="AB56" s="45" t="n"/>
+      <c r="AC56" s="45" t="n"/>
+      <c r="AD56" s="45" t="n"/>
+      <c r="AE56" s="45" t="n"/>
+      <c r="AF56" s="45" t="n"/>
+      <c r="AG56" s="46" t="n"/>
+      <c r="AH56" s="46" t="n"/>
+      <c r="AI56" s="47" t="n"/>
+      <c r="AJ56" s="47" t="n"/>
+      <c r="AK56" s="47" t="n"/>
+    </row>
+    <row r="57" ht="15" customHeight="1" s="29">
+      <c r="A57" s="45" t="inlineStr">
+        <is>
+          <t>NataliaOno</t>
+        </is>
+      </c>
+      <c r="B57" s="45" t="n"/>
+      <c r="Q57" s="45" t="n">
+        <v>437</v>
+      </c>
+      <c r="R57" s="45" t="n">
+        <v>13</v>
+      </c>
+      <c r="S57" s="45" t="n">
+        <v>36</v>
+      </c>
+      <c r="T57" s="45" t="n">
+        <v>367</v>
+      </c>
+      <c r="U57" s="45" t="n">
+        <v>169</v>
+      </c>
+      <c r="V57" s="45" t="n">
+        <v>1134</v>
+      </c>
+      <c r="W57" s="45" t="n">
+        <v>1325</v>
+      </c>
+      <c r="X57" s="46" t="n">
+        <v>169</v>
+      </c>
+      <c r="Y57" s="46" t="n">
+        <v>240</v>
+      </c>
+      <c r="Z57" s="45" t="n">
+        <v>270</v>
+      </c>
+      <c r="AA57" s="45" t="n">
+        <v>597</v>
+      </c>
+      <c r="AB57" s="45" t="n">
+        <v>670</v>
+      </c>
+      <c r="AC57" s="45" t="n">
+        <v>1134</v>
+      </c>
+      <c r="AD57" s="45" t="n">
+        <v>1325</v>
+      </c>
+      <c r="AE57" s="45" t="n">
+        <v>1620</v>
+      </c>
+      <c r="AF57" s="45" t="n">
+        <v>1650</v>
+      </c>
+      <c r="AG57" s="46" t="n">
+        <v>357</v>
+      </c>
+      <c r="AH57" s="46" t="n">
+        <v>1023</v>
+      </c>
+      <c r="AI57" s="47" t="n">
+        <v>0.3489736070381232</v>
+      </c>
+      <c r="AJ57" s="47" t="n">
+        <v>-20.9</v>
+      </c>
+      <c r="AK57" s="47" t="n">
+        <v>30.7</v>
+      </c>
+    </row>
     <row r="58" ht="15" customHeight="1" s="29"/>
     <row r="59" ht="15" customHeight="1" s="29"/>
     <row r="60" ht="15" customHeight="1" s="29"/>

</xml_diff>